<commit_message>
Interanual y mayor incremento mensual
</commit_message>
<xml_diff>
--- a/indecnacional.xlsx
+++ b/indecnacional.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -3208,6 +3208,50 @@
         <v>44621</v>
       </c>
     </row>
+    <row r="65">
+      <c r="A65">
+        <v>6</v>
+      </c>
+      <c r="B65">
+        <v>5.9</v>
+      </c>
+      <c r="C65">
+        <v>3.3</v>
+      </c>
+      <c r="D65">
+        <v>9.9</v>
+      </c>
+      <c r="E65">
+        <v>4.6</v>
+      </c>
+      <c r="F65">
+        <v>5.5</v>
+      </c>
+      <c r="G65">
+        <v>6.4</v>
+      </c>
+      <c r="H65">
+        <v>5.3</v>
+      </c>
+      <c r="I65">
+        <v>3.7</v>
+      </c>
+      <c r="J65">
+        <v>5.2</v>
+      </c>
+      <c r="K65">
+        <v>3.7</v>
+      </c>
+      <c r="L65">
+        <v>7.3</v>
+      </c>
+      <c r="M65">
+        <v>5.3</v>
+      </c>
+      <c r="N65" s="2">
+        <v>44652</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modif index.Rmd source download data
</commit_message>
<xml_diff>
--- a/indecnacional.xlsx
+++ b/indecnacional.xlsx
@@ -1,24 +1,122 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxig\Desktop\Carpetas\Trabajos en R\Shiny Indec App\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFEA153-D977-4364-BED4-816464F5CF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
+  <si>
+    <t>Nivel general</t>
+  </si>
+  <si>
+    <t>Alimentos y bebidas</t>
+  </si>
+  <si>
+    <t>Bebidas alcohólicas y tabaco</t>
+  </si>
+  <si>
+    <t>Prendias y Calzado</t>
+  </si>
+  <si>
+    <t>Vivienda Agua y Elec</t>
+  </si>
+  <si>
+    <t>Equip y Mant del Hogar</t>
+  </si>
+  <si>
+    <t>Salud</t>
+  </si>
+  <si>
+    <t>Transporte</t>
+  </si>
+  <si>
+    <t>Comunicación</t>
+  </si>
+  <si>
+    <t>Recreación y cultura</t>
+  </si>
+  <si>
+    <t>Educación</t>
+  </si>
+  <si>
+    <t>Restaurantes y hoteles</t>
+  </si>
+  <si>
+    <t>Bienes y servicios varios</t>
+  </si>
+  <si>
+    <t>periodos</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>Mar</t>
+  </si>
+  <si>
+    <t>Apr</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Jun</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Aug</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Oct</t>
+  </si>
+  <si>
+    <t>Nov</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -67,11 +165,19 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -113,7 +219,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -145,9 +251,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -179,6 +303,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,104 +496,72 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E56" sqref="E56"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.7265625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Nivel general</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Alimentos y bebidas</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Bebidas alcohólicas y tabaco</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Prendias y Calzado</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Vivienda Agua y Elec</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Equip y Mant del Hogar</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Salud</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Transporte</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Comunicación</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Recreación y cultura</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Educación</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Restaurantes y hoteles</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Bienes y servicios varios</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>periodos</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>year</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>Mes</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>month</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1.6</v>
       </c>
@@ -500,13 +610,11 @@
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="Q2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2.1</v>
       </c>
@@ -532,7 +640,7 @@
         <v>1.9</v>
       </c>
       <c r="I3">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="J3">
         <v>0.6</v>
@@ -555,13 +663,11 @@
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="Q3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2.4</v>
       </c>
@@ -610,18 +716,16 @@
       <c r="P4">
         <v>3</v>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2.7</v>
       </c>
       <c r="B5">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C5">
         <v>2.4</v>
@@ -633,7 +737,7 @@
         <v>5.9</v>
       </c>
       <c r="F5">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G5">
         <v>1.8</v>
@@ -665,13 +769,11 @@
       <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="Q5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -720,13 +822,11 @@
       <c r="P6">
         <v>5</v>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+      <c r="Q6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1.2</v>
       </c>
@@ -755,7 +855,7 @@
         <v>1.2</v>
       </c>
       <c r="J7">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -775,18 +875,16 @@
       <c r="P7">
         <v>6</v>
       </c>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
+      <c r="Q7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1.7</v>
       </c>
       <c r="B8">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -804,7 +902,7 @@
         <v>3.3</v>
       </c>
       <c r="H8">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I8">
         <v>0.9</v>
@@ -830,13 +928,11 @@
       <c r="P8">
         <v>7</v>
       </c>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="Q8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>1.4</v>
       </c>
@@ -850,7 +946,7 @@
         <v>-0.6</v>
       </c>
       <c r="E9">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -859,7 +955,7 @@
         <v>2.5</v>
       </c>
       <c r="H9">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I9">
         <v>1.5</v>
@@ -885,13 +981,11 @@
       <c r="P9">
         <v>8</v>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
+      <c r="Q9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1.9</v>
       </c>
@@ -917,7 +1011,7 @@
         <v>0.8</v>
       </c>
       <c r="I10">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J10">
         <v>2.7</v>
@@ -940,13 +1034,11 @@
       <c r="P10">
         <v>9</v>
       </c>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
+      <c r="Q10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>1.5</v>
       </c>
@@ -966,7 +1058,7 @@
         <v>0.7</v>
       </c>
       <c r="G11">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H11">
         <v>1.3</v>
@@ -995,13 +1087,11 @@
       <c r="P11">
         <v>10</v>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
+      <c r="Q11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>1.4</v>
       </c>
@@ -1009,7 +1099,7 @@
         <v>1.2</v>
       </c>
       <c r="C12">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D12">
         <v>1.3</v>
@@ -1050,13 +1140,11 @@
       <c r="P12">
         <v>11</v>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>3.1</v>
       </c>
@@ -1094,7 +1182,7 @@
         <v>1.8</v>
       </c>
       <c r="M13">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="N13" s="2">
         <v>43070</v>
@@ -1105,13 +1193,11 @@
       <c r="P13">
         <v>12</v>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
+      <c r="Q13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1.8</v>
       </c>
@@ -1119,7 +1205,7 @@
         <v>2.1</v>
       </c>
       <c r="C14">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D14">
         <v>-0.8</v>
@@ -1134,7 +1220,7 @@
         <v>1.8</v>
       </c>
       <c r="H14">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I14">
         <v>1.9</v>
@@ -1160,18 +1246,16 @@
       <c r="P14">
         <v>1</v>
       </c>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
+      <c r="Q14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2.4</v>
       </c>
       <c r="B15">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C15">
         <v>1.7</v>
@@ -1186,7 +1270,7 @@
         <v>1.7</v>
       </c>
       <c r="G15">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H15">
         <v>4.5</v>
@@ -1215,24 +1299,22 @@
       <c r="P15">
         <v>2</v>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
+      <c r="Q15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B16">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C16">
         <v>0.7</v>
       </c>
       <c r="D16">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E16">
         <v>0.6</v>
@@ -1270,13 +1352,11 @@
       <c r="P16">
         <v>3</v>
       </c>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
+      <c r="Q16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2.7</v>
       </c>
@@ -1311,7 +1391,7 @@
         <v>0.8</v>
       </c>
       <c r="L17">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="M17">
         <v>1.7</v>
@@ -1325,13 +1405,11 @@
       <c r="P17">
         <v>4</v>
       </c>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
+      <c r="Q17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2.1</v>
       </c>
@@ -1348,10 +1426,10 @@
         <v>-0.7</v>
       </c>
       <c r="F18">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G18">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H18">
         <v>1.9</v>
@@ -1380,13 +1458,11 @@
       <c r="P18">
         <v>5</v>
       </c>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
+      <c r="Q18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>3.7</v>
       </c>
@@ -1435,13 +1511,11 @@
       <c r="P19">
         <v>6</v>
       </c>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
+      <c r="Q19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3.1</v>
       </c>
@@ -1470,7 +1544,7 @@
         <v>0.6</v>
       </c>
       <c r="J20">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="K20">
         <v>1.8</v>
@@ -1490,13 +1564,11 @@
       <c r="P20">
         <v>7</v>
       </c>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
+      <c r="Q20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>3.9</v>
       </c>
@@ -1516,7 +1588,7 @@
         <v>3.1</v>
       </c>
       <c r="G21">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H21">
         <v>4</v>
@@ -1534,7 +1606,7 @@
         <v>2.4</v>
       </c>
       <c r="M21">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N21" s="2">
         <v>43313</v>
@@ -1545,13 +1617,11 @@
       <c r="P21">
         <v>8</v>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
+      <c r="Q21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>6.5</v>
       </c>
@@ -1559,16 +1629,16 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D22">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="E22">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F22">
-        <v>9.699999999999999</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="G22">
         <v>4.5</v>
@@ -1600,13 +1670,11 @@
       <c r="P22">
         <v>9</v>
       </c>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
+      <c r="Q22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>5.4</v>
       </c>
@@ -1614,13 +1682,13 @@
         <v>5.9</v>
       </c>
       <c r="C23">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23">
-        <v>8.800000000000001</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="F23">
         <v>4.3</v>
@@ -1655,13 +1723,11 @@
       <c r="P23">
         <v>10</v>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
+      <c r="Q23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1669,10 +1735,10 @@
         <v>3.4</v>
       </c>
       <c r="C24">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D24">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E24">
         <v>2.1</v>
@@ -1699,7 +1765,7 @@
         <v>2.6</v>
       </c>
       <c r="M24">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N24" s="2">
         <v>43405</v>
@@ -1710,13 +1776,11 @@
       <c r="P24">
         <v>11</v>
       </c>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
+      <c r="Q24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2.6</v>
       </c>
@@ -1727,7 +1791,7 @@
         <v>1.4</v>
       </c>
       <c r="D25">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1765,13 +1829,11 @@
       <c r="P25">
         <v>12</v>
       </c>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
+      <c r="Q25" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2.9</v>
       </c>
@@ -1820,13 +1882,11 @@
       <c r="P26">
         <v>1</v>
       </c>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
+      <c r="Q26" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>3.8</v>
       </c>
@@ -1849,13 +1909,13 @@
         <v>3.2</v>
       </c>
       <c r="H27">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I27">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J27">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K27">
         <v>1.7</v>
@@ -1875,13 +1935,11 @@
       <c r="P27">
         <v>2</v>
       </c>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
+      <c r="Q27" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>4.7</v>
       </c>
@@ -1889,7 +1947,7 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D28">
         <v>6.6</v>
@@ -1907,13 +1965,13 @@
         <v>4.2</v>
       </c>
       <c r="I28">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="J28">
         <v>2</v>
       </c>
       <c r="K28">
-        <v>17.9</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="L28">
         <v>4.3</v>
@@ -1930,13 +1988,11 @@
       <c r="P28">
         <v>3</v>
       </c>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
+      <c r="Q28" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>3.4</v>
       </c>
@@ -1953,13 +2009,13 @@
         <v>2.9</v>
       </c>
       <c r="F29">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G29">
         <v>3.5</v>
       </c>
       <c r="H29">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="I29">
         <v>3.5</v>
@@ -1971,7 +2027,7 @@
         <v>1.5</v>
       </c>
       <c r="L29">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -1985,13 +2041,11 @@
       <c r="P29">
         <v>4</v>
       </c>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
+      <c r="Q29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>3.1</v>
       </c>
@@ -1999,7 +2053,7 @@
         <v>2.4</v>
       </c>
       <c r="C30">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D30">
         <v>3.4</v>
@@ -2011,7 +2065,7 @@
         <v>3.2</v>
       </c>
       <c r="G30">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="H30">
         <v>3.5</v>
@@ -2026,7 +2080,7 @@
         <v>3.3</v>
       </c>
       <c r="L30">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M30">
         <v>2.8</v>
@@ -2040,13 +2094,11 @@
       <c r="P30">
         <v>5</v>
       </c>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
+      <c r="Q30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2.7</v>
       </c>
@@ -2095,18 +2147,16 @@
       <c r="P31">
         <v>6</v>
       </c>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
+      <c r="Q31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B32">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="C32">
         <v>0.9</v>
@@ -2115,16 +2165,16 @@
         <v>0.3</v>
       </c>
       <c r="E32">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F32">
         <v>2.5</v>
       </c>
       <c r="G32">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H32">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I32">
         <v>0.2</v>
@@ -2150,13 +2200,11 @@
       <c r="P32">
         <v>7</v>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
+      <c r="Q32" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2164,7 +2212,7 @@
         <v>4.5</v>
       </c>
       <c r="C33">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="D33">
         <v>3.1</v>
@@ -2194,7 +2242,7 @@
         <v>3.6</v>
       </c>
       <c r="M33">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="N33" s="2">
         <v>43678</v>
@@ -2205,13 +2253,11 @@
       <c r="P33">
         <v>8</v>
       </c>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
+      <c r="Q33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>5.9</v>
       </c>
@@ -2231,7 +2277,7 @@
         <v>7.4</v>
       </c>
       <c r="G34">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="H34">
         <v>4.7</v>
@@ -2249,7 +2295,7 @@
         <v>5.2</v>
       </c>
       <c r="M34">
-        <v>8.199999999999999</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="N34" s="2">
         <v>43709</v>
@@ -2260,13 +2306,11 @@
       <c r="P34">
         <v>9</v>
       </c>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
+      <c r="Q34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -2315,13 +2359,11 @@
       <c r="P35">
         <v>10</v>
       </c>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
+      <c r="Q35" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>4.3</v>
       </c>
@@ -2332,7 +2374,7 @@
         <v>5.6</v>
       </c>
       <c r="D36">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="E36">
         <v>1.5</v>
@@ -2344,7 +2386,7 @@
         <v>6.3</v>
       </c>
       <c r="H36">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I36">
         <v>7.4</v>
@@ -2353,13 +2395,13 @@
         <v>3.4</v>
       </c>
       <c r="K36">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="L36">
         <v>3.3</v>
       </c>
       <c r="M36">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="N36" s="2">
         <v>43770</v>
@@ -2370,13 +2412,11 @@
       <c r="P36">
         <v>11</v>
       </c>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
+      <c r="Q36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>3.7</v>
       </c>
@@ -2425,15 +2465,13 @@
       <c r="P37">
         <v>12</v>
       </c>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
+      <c r="Q37" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A38">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="B38">
         <v>4.7</v>
@@ -2442,7 +2480,7 @@
         <v>4.3</v>
       </c>
       <c r="D38">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E38">
         <v>0.6</v>
@@ -2480,13 +2518,11 @@
       <c r="P38">
         <v>1</v>
       </c>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
+      <c r="Q38" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2512,10 +2548,10 @@
         <v>1.6</v>
       </c>
       <c r="I39">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="J39">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K39">
         <v>1.4</v>
@@ -2535,13 +2571,11 @@
       <c r="P39">
         <v>2</v>
       </c>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
+      <c r="Q39" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>3.3</v>
       </c>
@@ -2567,7 +2601,7 @@
         <v>1.6</v>
       </c>
       <c r="I40">
-        <v>8.300000000000001</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="J40">
         <v>2.5</v>
@@ -2576,7 +2610,7 @@
         <v>17.5</v>
       </c>
       <c r="L40">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M40">
         <v>2</v>
@@ -2590,13 +2624,11 @@
       <c r="P40">
         <v>3</v>
       </c>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
+      <c r="Q40" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1.5</v>
       </c>
@@ -2622,10 +2654,10 @@
         <v>1.3</v>
       </c>
       <c r="I41">
-        <v>-4.1</v>
+        <v>-4.0999999999999996</v>
       </c>
       <c r="J41">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K41">
         <v>-1.5</v>
@@ -2645,13 +2677,11 @@
       <c r="P41">
         <v>4</v>
       </c>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
+      <c r="Q41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1.5</v>
       </c>
@@ -2671,10 +2701,10 @@
         <v>2.8</v>
       </c>
       <c r="G42">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H42">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="I42">
         <v>0.3</v>
@@ -2700,15 +2730,13 @@
       <c r="P42">
         <v>5</v>
       </c>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
+      <c r="Q42" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A43">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2723,10 +2751,10 @@
         <v>0.9</v>
       </c>
       <c r="F43">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G43">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H43">
         <v>1.8</v>
@@ -2741,7 +2769,7 @@
         <v>0.4</v>
       </c>
       <c r="L43">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="M43">
         <v>0.3</v>
@@ -2755,13 +2783,11 @@
       <c r="P43">
         <v>6</v>
       </c>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
+      <c r="Q43" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1.9</v>
       </c>
@@ -2781,7 +2807,7 @@
         <v>3.9</v>
       </c>
       <c r="G44">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H44">
         <v>1.8</v>
@@ -2799,7 +2825,7 @@
         <v>1.9</v>
       </c>
       <c r="M44">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="N44" s="2">
         <v>44013</v>
@@ -2810,13 +2836,11 @@
       <c r="P44">
         <v>7</v>
       </c>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
+      <c r="Q44" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2.7</v>
       </c>
@@ -2827,10 +2851,10 @@
         <v>1.3</v>
       </c>
       <c r="D45">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E45">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F45">
         <v>3.5</v>
@@ -2865,13 +2889,11 @@
       <c r="P45">
         <v>8</v>
       </c>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
+      <c r="Q45" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2.8</v>
       </c>
@@ -2920,13 +2942,11 @@
       <c r="P46">
         <v>9</v>
       </c>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
+      <c r="Q46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>3.8</v>
       </c>
@@ -2940,7 +2960,7 @@
         <v>6.2</v>
       </c>
       <c r="E47">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F47">
         <v>4.5</v>
@@ -2975,13 +2995,11 @@
       <c r="P47">
         <v>10</v>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
+      <c r="Q47" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>3.2</v>
       </c>
@@ -3010,7 +3028,7 @@
         <v>-0.6</v>
       </c>
       <c r="J48">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="K48">
         <v>0.4</v>
@@ -3030,18 +3048,16 @@
       <c r="P48">
         <v>11</v>
       </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
+      <c r="Q48" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C49">
         <v>3.4</v>
@@ -3059,7 +3075,7 @@
         <v>5.2</v>
       </c>
       <c r="H49">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -3071,7 +3087,7 @@
         <v>0</v>
       </c>
       <c r="L49">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="M49">
         <v>1.7</v>
@@ -3085,13 +3101,11 @@
       <c r="P49">
         <v>12</v>
       </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
+      <c r="Q49" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>4</v>
       </c>
@@ -3105,7 +3119,7 @@
         <v>1.4</v>
       </c>
       <c r="E50">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F50">
         <v>3</v>
@@ -3114,7 +3128,7 @@
         <v>3.4</v>
       </c>
       <c r="H50">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="I50">
         <v>15.1</v>
@@ -3140,13 +3154,11 @@
       <c r="P50">
         <v>1</v>
       </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
+      <c r="Q50" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>3.6</v>
       </c>
@@ -3163,7 +3175,7 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G51">
         <v>3.5</v>
@@ -3175,7 +3187,7 @@
         <v>1.8</v>
       </c>
       <c r="J51">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K51">
         <v>0.1</v>
@@ -3195,18 +3207,16 @@
       <c r="P51">
         <v>2</v>
       </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
+      <c r="Q51" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>4.8</v>
       </c>
       <c r="B52">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C52">
         <v>6.4</v>
@@ -3239,7 +3249,7 @@
         <v>3.1</v>
       </c>
       <c r="M52">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N52" s="2">
         <v>44256</v>
@@ -3250,15 +3260,13 @@
       <c r="P52">
         <v>3</v>
       </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
+      <c r="Q52" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A53">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B53">
         <v>4.3</v>
@@ -3305,13 +3313,11 @@
       <c r="P53">
         <v>4</v>
       </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
+      <c r="Q53" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>3.3</v>
       </c>
@@ -3343,7 +3349,7 @@
         <v>3.1</v>
       </c>
       <c r="K54">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="L54">
         <v>3.7</v>
@@ -3360,13 +3366,11 @@
       <c r="P54">
         <v>5</v>
       </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
+      <c r="Q54" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>3.2</v>
       </c>
@@ -3395,10 +3399,10 @@
         <v>7</v>
       </c>
       <c r="J55">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="K55">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L55">
         <v>3.1</v>
@@ -3415,13 +3419,11 @@
       <c r="P55">
         <v>6</v>
       </c>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
+      <c r="Q55" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3444,7 +3446,7 @@
         <v>3.8</v>
       </c>
       <c r="H56">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="I56">
         <v>0.4</v>
@@ -3470,13 +3472,11 @@
       <c r="P56">
         <v>7</v>
       </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
+      <c r="Q56" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2.5</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>3.4</v>
       </c>
       <c r="E57">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F57">
         <v>3.3</v>
@@ -3525,13 +3525,11 @@
       <c r="P57">
         <v>8</v>
       </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
+      <c r="Q57" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>3.5</v>
       </c>
@@ -3566,10 +3564,10 @@
         <v>3.1</v>
       </c>
       <c r="L58">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M58">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="N58" s="2">
         <v>44440</v>
@@ -3580,13 +3578,11 @@
       <c r="P58">
         <v>9</v>
       </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
+      <c r="Q58" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>3.5</v>
       </c>
@@ -3594,10 +3590,10 @@
         <v>3.4</v>
       </c>
       <c r="C59">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="D59">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="E59">
         <v>2.5</v>
@@ -3612,7 +3608,7 @@
         <v>3.1</v>
       </c>
       <c r="I59">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="J59">
         <v>4</v>
@@ -3621,7 +3617,7 @@
         <v>1.4</v>
       </c>
       <c r="L59">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="M59">
         <v>3.3</v>
@@ -3635,13 +3631,11 @@
       <c r="P59">
         <v>10</v>
       </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
+      <c r="Q59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2.5</v>
       </c>
@@ -3649,13 +3643,13 @@
         <v>2.1</v>
       </c>
       <c r="C60">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D60">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="E60">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F60">
         <v>2.7</v>
@@ -3664,7 +3658,7 @@
         <v>2.4</v>
       </c>
       <c r="H60">
-        <v>2.2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I60">
         <v>0.8</v>
@@ -3690,13 +3684,11 @@
       <c r="P60">
         <v>11</v>
       </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
+      <c r="Q60" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>3.8</v>
       </c>
@@ -3719,7 +3711,7 @@
         <v>0.5</v>
       </c>
       <c r="H61">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I61">
         <v>1.8</v>
@@ -3745,18 +3737,16 @@
       <c r="P61">
         <v>12</v>
       </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
+      <c r="Q61" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>3.9</v>
       </c>
       <c r="B62">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="C62">
         <v>1.8</v>
@@ -3771,7 +3761,7 @@
         <v>3.3</v>
       </c>
       <c r="G62">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H62">
         <v>2.8</v>
@@ -3800,13 +3790,11 @@
       <c r="P62">
         <v>1</v>
       </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
+      <c r="Q62" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>4.7</v>
       </c>
@@ -3823,19 +3811,19 @@
         <v>2.8</v>
       </c>
       <c r="F63">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G63">
         <v>3.6</v>
       </c>
       <c r="H63">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I63">
         <v>1.5</v>
       </c>
       <c r="J63">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="K63">
         <v>2.6</v>
@@ -3855,13 +3843,11 @@
       <c r="P63">
         <v>2</v>
       </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
+      <c r="Q63" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>6.7</v>
       </c>
@@ -3878,7 +3864,7 @@
         <v>7.7</v>
       </c>
       <c r="F64">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G64">
         <v>5</v>
@@ -3910,13 +3896,11 @@
       <c r="P64">
         <v>3</v>
       </c>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>Mar</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
+      <c r="Q64" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>6</v>
       </c>
@@ -3930,7 +3914,7 @@
         <v>9.9</v>
       </c>
       <c r="E65">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F65">
         <v>5.5</v>
@@ -3965,18 +3949,16 @@
       <c r="P65">
         <v>4</v>
       </c>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>Apr</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
+      <c r="Q65" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A66">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B66">
-        <v>4.4</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="C66">
         <v>5.7</v>
@@ -4009,7 +3991,7 @@
         <v>5.7</v>
       </c>
       <c r="M66">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="N66" s="2">
         <v>44682</v>
@@ -4020,18 +4002,16 @@
       <c r="P66">
         <v>5</v>
       </c>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>May</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
+      <c r="Q66" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>5.3</v>
       </c>
       <c r="B67">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C67">
         <v>6.7</v>
@@ -4075,13 +4055,11 @@
       <c r="P67">
         <v>6</v>
       </c>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>Jun</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
+      <c r="Q67" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>7.4</v>
       </c>
@@ -4095,7 +4073,7 @@
         <v>8.5</v>
       </c>
       <c r="E68">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F68">
         <v>10.3</v>
@@ -4116,7 +4094,7 @@
         <v>6.1</v>
       </c>
       <c r="L68">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="M68">
         <v>8.1</v>
@@ -4130,13 +4108,11 @@
       <c r="P68">
         <v>7</v>
       </c>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>Jul</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
+      <c r="Q68" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>7</v>
       </c>
@@ -4162,7 +4138,7 @@
         <v>6.8</v>
       </c>
       <c r="I69">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="J69">
         <v>5</v>
@@ -4174,7 +4150,7 @@
         <v>6.7</v>
       </c>
       <c r="M69">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="N69" s="2">
         <v>44774</v>
@@ -4185,13 +4161,11 @@
       <c r="P69">
         <v>8</v>
       </c>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>Aug</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
+      <c r="Q69" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>6.2</v>
       </c>
@@ -4240,13 +4214,11 @@
       <c r="P70">
         <v>9</v>
       </c>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>Sep</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
+      <c r="Q70" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>6.3</v>
       </c>
@@ -4263,7 +4235,7 @@
         <v>7.5</v>
       </c>
       <c r="F71">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="G71">
         <v>7.1</v>
@@ -4295,15 +4267,13 @@
       <c r="P71">
         <v>10</v>
       </c>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>Oct</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
+      <c r="Q71" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A72">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="B72">
         <v>3.5</v>
@@ -4315,13 +4285,13 @@
         <v>4.5</v>
       </c>
       <c r="E72">
-        <v>8.699999999999999</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="F72">
         <v>5.4</v>
       </c>
       <c r="G72">
-        <v>4.1</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H72">
         <v>6.1</v>
@@ -4350,15 +4320,13 @@
       <c r="P72">
         <v>11</v>
       </c>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>Nov</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
+      <c r="Q72" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A73">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="B73">
         <v>4.7</v>
@@ -4385,7 +4353,7 @@
         <v>3.4</v>
       </c>
       <c r="J73">
-        <v>4.6</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="K73">
         <v>3.9</v>
@@ -4405,13 +4373,11 @@
       <c r="P73">
         <v>12</v>
       </c>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>Dec</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
+      <c r="Q73" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>6</v>
       </c>
@@ -4422,7 +4388,7 @@
         <v>7.3</v>
       </c>
       <c r="D74">
-        <v>2.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E74">
         <v>8</v>
@@ -4431,7 +4397,7 @@
         <v>5.4</v>
       </c>
       <c r="G74">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="H74">
         <v>5.9</v>
@@ -4443,7 +4409,7 @@
         <v>9</v>
       </c>
       <c r="K74">
-        <v>1.1</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="L74">
         <v>6.2</v>
@@ -4460,18 +4426,16 @@
       <c r="P74">
         <v>1</v>
       </c>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>Jan</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
+      <c r="Q74" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>6.6</v>
       </c>
       <c r="B75">
-        <v>9.800000000000001</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="C75">
         <v>5.2</v>
@@ -4483,13 +4447,13 @@
         <v>4.8</v>
       </c>
       <c r="F75">
-        <v>5.1</v>
+        <v>5.0999999999999996</v>
       </c>
       <c r="G75">
         <v>5.3</v>
       </c>
       <c r="H75">
-        <v>4.9</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="I75">
         <v>7.8</v>
@@ -4515,10 +4479,8 @@
       <c r="P75">
         <v>2</v>
       </c>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>Feb</t>
-        </is>
+      <c r="Q75" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
set docker environment + new workflow
</commit_message>
<xml_diff>
--- a/indecnacional.xlsx
+++ b/indecnacional.xlsx
@@ -1,122 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxig\Desktop\Carpetas\Trabajos en R\Shiny Indec App\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FFEA153-D977-4364-BED4-816464F5CF80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="29">
-  <si>
-    <t>Nivel general</t>
-  </si>
-  <si>
-    <t>Alimentos y bebidas</t>
-  </si>
-  <si>
-    <t>Bebidas alcohólicas y tabaco</t>
-  </si>
-  <si>
-    <t>Prendias y Calzado</t>
-  </si>
-  <si>
-    <t>Vivienda Agua y Elec</t>
-  </si>
-  <si>
-    <t>Equip y Mant del Hogar</t>
-  </si>
-  <si>
-    <t>Salud</t>
-  </si>
-  <si>
-    <t>Transporte</t>
-  </si>
-  <si>
-    <t>Comunicación</t>
-  </si>
-  <si>
-    <t>Recreación y cultura</t>
-  </si>
-  <si>
-    <t>Educación</t>
-  </si>
-  <si>
-    <t>Restaurantes y hoteles</t>
-  </si>
-  <si>
-    <t>Bienes y servicios varios</t>
-  </si>
-  <si>
-    <t>periodos</t>
-  </si>
-  <si>
-    <t>year</t>
-  </si>
-  <si>
-    <t>Mes</t>
-  </si>
-  <si>
-    <t>month</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Feb</t>
-  </si>
-  <si>
-    <t>Mar</t>
-  </si>
-  <si>
-    <t>Apr</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>Jun</t>
-  </si>
-  <si>
-    <t>Jul</t>
-  </si>
-  <si>
-    <t>Aug</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,19 +67,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -219,7 +113,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,27 +145,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -303,24 +179,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,72 +354,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="14" max="14" width="20.7265625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Nivel general</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Alimentos y bebidas</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Bebidas alcohólicas y tabaco</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Prendias y Calzado</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Vivienda Agua y Elec</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Equip y Mant del Hogar</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Salud</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Transporte</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Comunicación</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Recreación y cultura</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Educación</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Restaurantes y hoteles</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Bienes y servicios varios</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>periodos</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>year</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Mes</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>month</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
       <c r="A2">
         <v>1.6</v>
       </c>
@@ -610,11 +500,13 @@
       <c r="P2">
         <v>1</v>
       </c>
-      <c r="Q2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3">
         <v>2.1</v>
       </c>
@@ -640,7 +532,7 @@
         <v>1.9</v>
       </c>
       <c r="I3">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="J3">
         <v>0.6</v>
@@ -663,11 +555,13 @@
       <c r="P3">
         <v>2</v>
       </c>
-      <c r="Q3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4">
         <v>2.4</v>
       </c>
@@ -716,16 +610,18 @@
       <c r="P4">
         <v>3</v>
       </c>
-      <c r="Q4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
       <c r="A5">
         <v>2.7</v>
       </c>
       <c r="B5">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="C5">
         <v>2.4</v>
@@ -737,7 +633,7 @@
         <v>5.9</v>
       </c>
       <c r="F5">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="G5">
         <v>1.8</v>
@@ -769,11 +665,13 @@
       <c r="P5">
         <v>4</v>
       </c>
-      <c r="Q5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6">
         <v>1.4</v>
       </c>
@@ -822,11 +720,13 @@
       <c r="P6">
         <v>5</v>
       </c>
-      <c r="Q6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7">
         <v>1.2</v>
       </c>
@@ -855,7 +755,7 @@
         <v>1.2</v>
       </c>
       <c r="J7">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -875,16 +775,18 @@
       <c r="P7">
         <v>6</v>
       </c>
-      <c r="Q7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8">
         <v>1.7</v>
       </c>
       <c r="B8">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="C8">
         <v>3</v>
@@ -902,7 +804,7 @@
         <v>3.3</v>
       </c>
       <c r="H8">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="I8">
         <v>0.9</v>
@@ -928,11 +830,13 @@
       <c r="P8">
         <v>7</v>
       </c>
-      <c r="Q8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
       <c r="A9">
         <v>1.4</v>
       </c>
@@ -946,7 +850,7 @@
         <v>-0.6</v>
       </c>
       <c r="E9">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -955,7 +859,7 @@
         <v>2.5</v>
       </c>
       <c r="H9">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="I9">
         <v>1.5</v>
@@ -981,11 +885,13 @@
       <c r="P9">
         <v>8</v>
       </c>
-      <c r="Q9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
       <c r="A10">
         <v>1.9</v>
       </c>
@@ -1011,7 +917,7 @@
         <v>0.8</v>
       </c>
       <c r="I10">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J10">
         <v>2.7</v>
@@ -1034,11 +940,13 @@
       <c r="P10">
         <v>9</v>
       </c>
-      <c r="Q10" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
       <c r="A11">
         <v>1.5</v>
       </c>
@@ -1058,7 +966,7 @@
         <v>0.7</v>
       </c>
       <c r="G11">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="H11">
         <v>1.3</v>
@@ -1087,11 +995,13 @@
       <c r="P11">
         <v>10</v>
       </c>
-      <c r="Q11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
       <c r="A12">
         <v>1.4</v>
       </c>
@@ -1099,7 +1009,7 @@
         <v>1.2</v>
       </c>
       <c r="C12">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="D12">
         <v>1.3</v>
@@ -1140,11 +1050,13 @@
       <c r="P12">
         <v>11</v>
       </c>
-      <c r="Q12" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
       <c r="A13">
         <v>3.1</v>
       </c>
@@ -1182,7 +1094,7 @@
         <v>1.8</v>
       </c>
       <c r="M13">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="N13" s="2">
         <v>43070</v>
@@ -1193,11 +1105,13 @@
       <c r="P13">
         <v>12</v>
       </c>
-      <c r="Q13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
       <c r="A14">
         <v>1.8</v>
       </c>
@@ -1205,7 +1119,7 @@
         <v>2.1</v>
       </c>
       <c r="C14">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="D14">
         <v>-0.8</v>
@@ -1220,7 +1134,7 @@
         <v>1.8</v>
       </c>
       <c r="H14">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="I14">
         <v>1.9</v>
@@ -1246,16 +1160,18 @@
       <c r="P14">
         <v>1</v>
       </c>
-      <c r="Q14" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
       <c r="A15">
         <v>2.4</v>
       </c>
       <c r="B15">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="C15">
         <v>1.7</v>
@@ -1270,7 +1186,7 @@
         <v>1.7</v>
       </c>
       <c r="G15">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="H15">
         <v>4.5</v>
@@ -1299,22 +1215,24 @@
       <c r="P15">
         <v>2</v>
       </c>
-      <c r="Q15" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
       <c r="A16">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="B16">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="C16">
         <v>0.7</v>
       </c>
       <c r="D16">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="E16">
         <v>0.6</v>
@@ -1352,11 +1270,13 @@
       <c r="P16">
         <v>3</v>
       </c>
-      <c r="Q16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
       <c r="A17">
         <v>2.7</v>
       </c>
@@ -1391,7 +1311,7 @@
         <v>0.8</v>
       </c>
       <c r="L17">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="M17">
         <v>1.7</v>
@@ -1405,11 +1325,13 @@
       <c r="P17">
         <v>4</v>
       </c>
-      <c r="Q17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
       <c r="A18">
         <v>2.1</v>
       </c>
@@ -1426,10 +1348,10 @@
         <v>-0.7</v>
       </c>
       <c r="F18">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="G18">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H18">
         <v>1.9</v>
@@ -1458,11 +1380,13 @@
       <c r="P18">
         <v>5</v>
       </c>
-      <c r="Q18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
       <c r="A19">
         <v>3.7</v>
       </c>
@@ -1511,11 +1435,13 @@
       <c r="P19">
         <v>6</v>
       </c>
-      <c r="Q19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
       <c r="A20">
         <v>3.1</v>
       </c>
@@ -1544,7 +1470,7 @@
         <v>0.6</v>
       </c>
       <c r="J20">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="K20">
         <v>1.8</v>
@@ -1564,11 +1490,13 @@
       <c r="P20">
         <v>7</v>
       </c>
-      <c r="Q20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
       <c r="A21">
         <v>3.9</v>
       </c>
@@ -1588,7 +1516,7 @@
         <v>3.1</v>
       </c>
       <c r="G21">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="H21">
         <v>4</v>
@@ -1606,7 +1534,7 @@
         <v>2.4</v>
       </c>
       <c r="M21">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="N21" s="2">
         <v>43313</v>
@@ -1617,11 +1545,13 @@
       <c r="P21">
         <v>8</v>
       </c>
-      <c r="Q21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
       <c r="A22">
         <v>6.5</v>
       </c>
@@ -1629,16 +1559,16 @@
         <v>7</v>
       </c>
       <c r="C22">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="D22">
-        <v>9.8000000000000007</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E22">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F22">
-        <v>9.6999999999999993</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="G22">
         <v>4.5</v>
@@ -1670,11 +1600,13 @@
       <c r="P22">
         <v>9</v>
       </c>
-      <c r="Q22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
       <c r="A23">
         <v>5.4</v>
       </c>
@@ -1682,13 +1614,13 @@
         <v>5.9</v>
       </c>
       <c r="C23">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="D23">
         <v>5</v>
       </c>
       <c r="E23">
-        <v>8.8000000000000007</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F23">
         <v>4.3</v>
@@ -1723,11 +1655,13 @@
       <c r="P23">
         <v>10</v>
       </c>
-      <c r="Q23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
       <c r="A24">
         <v>3.2</v>
       </c>
@@ -1735,10 +1669,10 @@
         <v>3.4</v>
       </c>
       <c r="C24">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="D24">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="E24">
         <v>2.1</v>
@@ -1765,7 +1699,7 @@
         <v>2.6</v>
       </c>
       <c r="M24">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="N24" s="2">
         <v>43405</v>
@@ -1776,11 +1710,13 @@
       <c r="P24">
         <v>11</v>
       </c>
-      <c r="Q24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
       <c r="A25">
         <v>2.6</v>
       </c>
@@ -1791,7 +1727,7 @@
         <v>1.4</v>
       </c>
       <c r="D25">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="E25">
         <v>3</v>
@@ -1829,11 +1765,13 @@
       <c r="P25">
         <v>12</v>
       </c>
-      <c r="Q25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
       <c r="A26">
         <v>2.9</v>
       </c>
@@ -1882,11 +1820,13 @@
       <c r="P26">
         <v>1</v>
       </c>
-      <c r="Q26" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
       <c r="A27">
         <v>3.8</v>
       </c>
@@ -1909,13 +1849,13 @@
         <v>3.2</v>
       </c>
       <c r="H27">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="I27">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J27">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="K27">
         <v>1.7</v>
@@ -1935,11 +1875,13 @@
       <c r="P27">
         <v>2</v>
       </c>
-      <c r="Q27" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
       <c r="A28">
         <v>4.7</v>
       </c>
@@ -1947,7 +1889,7 @@
         <v>6</v>
       </c>
       <c r="C28">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="D28">
         <v>6.6</v>
@@ -1965,13 +1907,13 @@
         <v>4.2</v>
       </c>
       <c r="I28">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="J28">
         <v>2</v>
       </c>
       <c r="K28">
-        <v>17.899999999999999</v>
+        <v>17.9</v>
       </c>
       <c r="L28">
         <v>4.3</v>
@@ -1988,11 +1930,13 @@
       <c r="P28">
         <v>3</v>
       </c>
-      <c r="Q28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
       <c r="A29">
         <v>3.4</v>
       </c>
@@ -2009,13 +1953,13 @@
         <v>2.9</v>
       </c>
       <c r="F29">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="G29">
         <v>3.5</v>
       </c>
       <c r="H29">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="I29">
         <v>3.5</v>
@@ -2027,7 +1971,7 @@
         <v>1.5</v>
       </c>
       <c r="L29">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="M29">
         <v>3</v>
@@ -2041,11 +1985,13 @@
       <c r="P29">
         <v>4</v>
       </c>
-      <c r="Q29" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
       <c r="A30">
         <v>3.1</v>
       </c>
@@ -2053,7 +1999,7 @@
         <v>2.4</v>
       </c>
       <c r="C30">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="D30">
         <v>3.4</v>
@@ -2065,7 +2011,7 @@
         <v>3.2</v>
       </c>
       <c r="G30">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="H30">
         <v>3.5</v>
@@ -2080,7 +2026,7 @@
         <v>3.3</v>
       </c>
       <c r="L30">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="M30">
         <v>2.8</v>
@@ -2094,11 +2040,13 @@
       <c r="P30">
         <v>5</v>
       </c>
-      <c r="Q30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
       <c r="A31">
         <v>2.7</v>
       </c>
@@ -2147,16 +2095,18 @@
       <c r="P31">
         <v>6</v>
       </c>
-      <c r="Q31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
       <c r="A32">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="B32">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="C32">
         <v>0.9</v>
@@ -2165,16 +2115,16 @@
         <v>0.3</v>
       </c>
       <c r="E32">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="F32">
         <v>2.5</v>
       </c>
       <c r="G32">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="H32">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="I32">
         <v>0.2</v>
@@ -2200,11 +2150,13 @@
       <c r="P32">
         <v>7</v>
       </c>
-      <c r="Q32" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2212,7 +2164,7 @@
         <v>4.5</v>
       </c>
       <c r="C33">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="D33">
         <v>3.1</v>
@@ -2242,7 +2194,7 @@
         <v>3.6</v>
       </c>
       <c r="M33">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="N33" s="2">
         <v>43678</v>
@@ -2253,11 +2205,13 @@
       <c r="P33">
         <v>8</v>
       </c>
-      <c r="Q33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
       <c r="A34">
         <v>5.9</v>
       </c>
@@ -2277,7 +2231,7 @@
         <v>7.4</v>
       </c>
       <c r="G34">
-        <v>8.3000000000000007</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="H34">
         <v>4.7</v>
@@ -2295,7 +2249,7 @@
         <v>5.2</v>
       </c>
       <c r="M34">
-        <v>8.1999999999999993</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="N34" s="2">
         <v>43709</v>
@@ -2306,11 +2260,13 @@
       <c r="P34">
         <v>9</v>
       </c>
-      <c r="Q34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
       <c r="A35">
         <v>3.3</v>
       </c>
@@ -2359,11 +2315,13 @@
       <c r="P35">
         <v>10</v>
       </c>
-      <c r="Q35" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
       <c r="A36">
         <v>4.3</v>
       </c>
@@ -2374,7 +2332,7 @@
         <v>5.6</v>
       </c>
       <c r="D36">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="E36">
         <v>1.5</v>
@@ -2386,7 +2344,7 @@
         <v>6.3</v>
       </c>
       <c r="H36">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I36">
         <v>7.4</v>
@@ -2395,13 +2353,13 @@
         <v>3.4</v>
       </c>
       <c r="K36">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="L36">
         <v>3.3</v>
       </c>
       <c r="M36">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="N36" s="2">
         <v>43770</v>
@@ -2412,11 +2370,13 @@
       <c r="P36">
         <v>11</v>
       </c>
-      <c r="Q36" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
       <c r="A37">
         <v>3.7</v>
       </c>
@@ -2465,13 +2425,15 @@
       <c r="P37">
         <v>12</v>
       </c>
-      <c r="Q37" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
       <c r="A38">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="B38">
         <v>4.7</v>
@@ -2480,7 +2442,7 @@
         <v>4.3</v>
       </c>
       <c r="D38">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="E38">
         <v>0.6</v>
@@ -2518,11 +2480,13 @@
       <c r="P38">
         <v>1</v>
       </c>
-      <c r="Q38" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
       <c r="A39">
         <v>2</v>
       </c>
@@ -2548,10 +2512,10 @@
         <v>1.6</v>
       </c>
       <c r="I39">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="J39">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="K39">
         <v>1.4</v>
@@ -2571,11 +2535,13 @@
       <c r="P39">
         <v>2</v>
       </c>
-      <c r="Q39" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
       <c r="A40">
         <v>3.3</v>
       </c>
@@ -2601,7 +2567,7 @@
         <v>1.6</v>
       </c>
       <c r="I40">
-        <v>8.3000000000000007</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="J40">
         <v>2.5</v>
@@ -2610,7 +2576,7 @@
         <v>17.5</v>
       </c>
       <c r="L40">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="M40">
         <v>2</v>
@@ -2624,11 +2590,13 @@
       <c r="P40">
         <v>3</v>
       </c>
-      <c r="Q40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
       <c r="A41">
         <v>1.5</v>
       </c>
@@ -2654,10 +2622,10 @@
         <v>1.3</v>
       </c>
       <c r="I41">
-        <v>-4.0999999999999996</v>
+        <v>-4.1</v>
       </c>
       <c r="J41">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="K41">
         <v>-1.5</v>
@@ -2677,11 +2645,13 @@
       <c r="P41">
         <v>4</v>
       </c>
-      <c r="Q41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
       <c r="A42">
         <v>1.5</v>
       </c>
@@ -2701,10 +2671,10 @@
         <v>2.8</v>
       </c>
       <c r="G42">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="H42">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="I42">
         <v>0.3</v>
@@ -2730,13 +2700,15 @@
       <c r="P42">
         <v>5</v>
       </c>
-      <c r="Q42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
       <c r="A43">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -2751,10 +2723,10 @@
         <v>0.9</v>
       </c>
       <c r="F43">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="G43">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H43">
         <v>1.8</v>
@@ -2769,7 +2741,7 @@
         <v>0.4</v>
       </c>
       <c r="L43">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="M43">
         <v>0.3</v>
@@ -2783,11 +2755,13 @@
       <c r="P43">
         <v>6</v>
       </c>
-      <c r="Q43" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
       <c r="A44">
         <v>1.9</v>
       </c>
@@ -2807,7 +2781,7 @@
         <v>3.9</v>
       </c>
       <c r="G44">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="H44">
         <v>1.8</v>
@@ -2825,7 +2799,7 @@
         <v>1.9</v>
       </c>
       <c r="M44">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="N44" s="2">
         <v>44013</v>
@@ -2836,11 +2810,13 @@
       <c r="P44">
         <v>7</v>
       </c>
-      <c r="Q44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
       <c r="A45">
         <v>2.7</v>
       </c>
@@ -2851,10 +2827,10 @@
         <v>1.3</v>
       </c>
       <c r="D45">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="E45">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F45">
         <v>3.5</v>
@@ -2889,11 +2865,13 @@
       <c r="P45">
         <v>8</v>
       </c>
-      <c r="Q45" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
       <c r="A46">
         <v>2.8</v>
       </c>
@@ -2942,11 +2920,13 @@
       <c r="P46">
         <v>9</v>
       </c>
-      <c r="Q46" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
       <c r="A47">
         <v>3.8</v>
       </c>
@@ -2960,7 +2940,7 @@
         <v>6.2</v>
       </c>
       <c r="E47">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="F47">
         <v>4.5</v>
@@ -2995,11 +2975,13 @@
       <c r="P47">
         <v>10</v>
       </c>
-      <c r="Q47" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
       <c r="A48">
         <v>3.2</v>
       </c>
@@ -3028,7 +3010,7 @@
         <v>-0.6</v>
       </c>
       <c r="J48">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="K48">
         <v>0.4</v>
@@ -3048,16 +3030,18 @@
       <c r="P48">
         <v>11</v>
       </c>
-      <c r="Q48" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
       <c r="A49">
         <v>4</v>
       </c>
       <c r="B49">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="C49">
         <v>3.4</v>
@@ -3075,7 +3059,7 @@
         <v>5.2</v>
       </c>
       <c r="H49">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="I49">
         <v>0</v>
@@ -3087,7 +3071,7 @@
         <v>0</v>
       </c>
       <c r="L49">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="M49">
         <v>1.7</v>
@@ -3101,11 +3085,13 @@
       <c r="P49">
         <v>12</v>
       </c>
-      <c r="Q49" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
       <c r="A50">
         <v>4</v>
       </c>
@@ -3119,7 +3105,7 @@
         <v>1.4</v>
       </c>
       <c r="E50">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="F50">
         <v>3</v>
@@ -3128,7 +3114,7 @@
         <v>3.4</v>
       </c>
       <c r="H50">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="I50">
         <v>15.1</v>
@@ -3154,11 +3140,13 @@
       <c r="P50">
         <v>1</v>
       </c>
-      <c r="Q50" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
       <c r="A51">
         <v>3.6</v>
       </c>
@@ -3175,7 +3163,7 @@
         <v>2</v>
       </c>
       <c r="F51">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="G51">
         <v>3.5</v>
@@ -3187,7 +3175,7 @@
         <v>1.8</v>
       </c>
       <c r="J51">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="K51">
         <v>0.1</v>
@@ -3207,16 +3195,18 @@
       <c r="P51">
         <v>2</v>
       </c>
-      <c r="Q51" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
       <c r="A52">
         <v>4.8</v>
       </c>
       <c r="B52">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="C52">
         <v>6.4</v>
@@ -3249,7 +3239,7 @@
         <v>3.1</v>
       </c>
       <c r="M52">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="N52" s="2">
         <v>44256</v>
@@ -3260,13 +3250,15 @@
       <c r="P52">
         <v>3</v>
       </c>
-      <c r="Q52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
       <c r="A53">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="B53">
         <v>4.3</v>
@@ -3313,11 +3305,13 @@
       <c r="P53">
         <v>4</v>
       </c>
-      <c r="Q53" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
       <c r="A54">
         <v>3.3</v>
       </c>
@@ -3349,7 +3343,7 @@
         <v>3.1</v>
       </c>
       <c r="K54">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="L54">
         <v>3.7</v>
@@ -3366,11 +3360,13 @@
       <c r="P54">
         <v>5</v>
       </c>
-      <c r="Q54" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
       <c r="A55">
         <v>3.2</v>
       </c>
@@ -3399,10 +3395,10 @@
         <v>7</v>
       </c>
       <c r="J55">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="K55">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="L55">
         <v>3.1</v>
@@ -3419,11 +3415,13 @@
       <c r="P55">
         <v>6</v>
       </c>
-      <c r="Q55" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3446,7 +3444,7 @@
         <v>3.8</v>
       </c>
       <c r="H56">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="I56">
         <v>0.4</v>
@@ -3472,11 +3470,13 @@
       <c r="P56">
         <v>7</v>
       </c>
-      <c r="Q56" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
       <c r="A57">
         <v>2.5</v>
       </c>
@@ -3490,7 +3490,7 @@
         <v>3.4</v>
       </c>
       <c r="E57">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="F57">
         <v>3.3</v>
@@ -3525,11 +3525,13 @@
       <c r="P57">
         <v>8</v>
       </c>
-      <c r="Q57" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
       <c r="A58">
         <v>3.5</v>
       </c>
@@ -3564,10 +3566,10 @@
         <v>3.1</v>
       </c>
       <c r="L58">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="M58">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="N58" s="2">
         <v>44440</v>
@@ -3578,11 +3580,13 @@
       <c r="P58">
         <v>9</v>
       </c>
-      <c r="Q58" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
       <c r="A59">
         <v>3.5</v>
       </c>
@@ -3590,10 +3594,10 @@
         <v>3.4</v>
       </c>
       <c r="C59">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="D59">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="E59">
         <v>2.5</v>
@@ -3608,7 +3612,7 @@
         <v>3.1</v>
       </c>
       <c r="I59">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="J59">
         <v>4</v>
@@ -3617,7 +3621,7 @@
         <v>1.4</v>
       </c>
       <c r="L59">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="M59">
         <v>3.3</v>
@@ -3631,11 +3635,13 @@
       <c r="P59">
         <v>10</v>
       </c>
-      <c r="Q59" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
       <c r="A60">
         <v>2.5</v>
       </c>
@@ -3643,13 +3649,13 @@
         <v>2.1</v>
       </c>
       <c r="C60">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="D60">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="E60">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="F60">
         <v>2.7</v>
@@ -3658,7 +3664,7 @@
         <v>2.4</v>
       </c>
       <c r="H60">
-        <v>2.2000000000000002</v>
+        <v>2.2</v>
       </c>
       <c r="I60">
         <v>0.8</v>
@@ -3684,11 +3690,13 @@
       <c r="P60">
         <v>11</v>
       </c>
-      <c r="Q60" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
       <c r="A61">
         <v>3.8</v>
       </c>
@@ -3711,7 +3719,7 @@
         <v>0.5</v>
       </c>
       <c r="H61">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="I61">
         <v>1.8</v>
@@ -3737,16 +3745,18 @@
       <c r="P61">
         <v>12</v>
       </c>
-      <c r="Q61" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
       <c r="A62">
         <v>3.9</v>
       </c>
       <c r="B62">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="C62">
         <v>1.8</v>
@@ -3761,7 +3771,7 @@
         <v>3.3</v>
       </c>
       <c r="G62">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="H62">
         <v>2.8</v>
@@ -3790,11 +3800,13 @@
       <c r="P62">
         <v>1</v>
       </c>
-      <c r="Q62" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
       <c r="A63">
         <v>4.7</v>
       </c>
@@ -3811,19 +3823,19 @@
         <v>2.8</v>
       </c>
       <c r="F63">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="G63">
         <v>3.6</v>
       </c>
       <c r="H63">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="I63">
         <v>1.5</v>
       </c>
       <c r="J63">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="K63">
         <v>2.6</v>
@@ -3843,11 +3855,13 @@
       <c r="P63">
         <v>2</v>
       </c>
-      <c r="Q63" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
       <c r="A64">
         <v>6.7</v>
       </c>
@@ -3864,7 +3878,7 @@
         <v>7.7</v>
       </c>
       <c r="F64">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="G64">
         <v>5</v>
@@ -3896,11 +3910,13 @@
       <c r="P64">
         <v>3</v>
       </c>
-      <c r="Q64" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
       <c r="A65">
         <v>6</v>
       </c>
@@ -3914,7 +3930,7 @@
         <v>9.9</v>
       </c>
       <c r="E65">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="F65">
         <v>5.5</v>
@@ -3949,16 +3965,18 @@
       <c r="P65">
         <v>4</v>
       </c>
-      <c r="Q65" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>Apr</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
       <c r="A66">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="B66">
-        <v>4.4000000000000004</v>
+        <v>4.4</v>
       </c>
       <c r="C66">
         <v>5.7</v>
@@ -3991,7 +4009,7 @@
         <v>5.7</v>
       </c>
       <c r="M66">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="N66" s="2">
         <v>44682</v>
@@ -4002,16 +4020,18 @@
       <c r="P66">
         <v>5</v>
       </c>
-      <c r="Q66" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>May</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
       <c r="A67">
         <v>5.3</v>
       </c>
       <c r="B67">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="C67">
         <v>6.7</v>
@@ -4055,11 +4075,13 @@
       <c r="P67">
         <v>6</v>
       </c>
-      <c r="Q67" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>Jun</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
       <c r="A68">
         <v>7.4</v>
       </c>
@@ -4073,7 +4095,7 @@
         <v>8.5</v>
       </c>
       <c r="E68">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="F68">
         <v>10.3</v>
@@ -4094,7 +4116,7 @@
         <v>6.1</v>
       </c>
       <c r="L68">
-        <v>9.8000000000000007</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="M68">
         <v>8.1</v>
@@ -4108,11 +4130,13 @@
       <c r="P68">
         <v>7</v>
       </c>
-      <c r="Q68" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>Jul</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
       <c r="A69">
         <v>7</v>
       </c>
@@ -4138,7 +4162,7 @@
         <v>6.8</v>
       </c>
       <c r="I69">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="J69">
         <v>5</v>
@@ -4150,7 +4174,7 @@
         <v>6.7</v>
       </c>
       <c r="M69">
-        <v>8.6999999999999993</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="N69" s="2">
         <v>44774</v>
@@ -4161,11 +4185,13 @@
       <c r="P69">
         <v>8</v>
       </c>
-      <c r="Q69" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>Aug</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
       <c r="A70">
         <v>6.2</v>
       </c>
@@ -4214,11 +4240,13 @@
       <c r="P70">
         <v>9</v>
       </c>
-      <c r="Q70" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>Sep</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
       <c r="A71">
         <v>6.3</v>
       </c>
@@ -4235,7 +4263,7 @@
         <v>7.5</v>
       </c>
       <c r="F71">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="G71">
         <v>7.1</v>
@@ -4267,13 +4295,15 @@
       <c r="P71">
         <v>10</v>
       </c>
-      <c r="Q71" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>Oct</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
       <c r="A72">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="B72">
         <v>3.5</v>
@@ -4285,13 +4315,13 @@
         <v>4.5</v>
       </c>
       <c r="E72">
-        <v>8.6999999999999993</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="F72">
         <v>5.4</v>
       </c>
       <c r="G72">
-        <v>4.0999999999999996</v>
+        <v>4.1</v>
       </c>
       <c r="H72">
         <v>6.1</v>
@@ -4320,13 +4350,15 @@
       <c r="P72">
         <v>11</v>
       </c>
-      <c r="Q72" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>Nov</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
       <c r="A73">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="B73">
         <v>4.7</v>
@@ -4353,7 +4385,7 @@
         <v>3.4</v>
       </c>
       <c r="J73">
-        <v>4.5999999999999996</v>
+        <v>4.6</v>
       </c>
       <c r="K73">
         <v>3.9</v>
@@ -4373,11 +4405,13 @@
       <c r="P73">
         <v>12</v>
       </c>
-      <c r="Q73" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>Dec</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
       <c r="A74">
         <v>6</v>
       </c>
@@ -4388,7 +4422,7 @@
         <v>7.3</v>
       </c>
       <c r="D74">
-        <v>2.2999999999999998</v>
+        <v>2.3</v>
       </c>
       <c r="E74">
         <v>8</v>
@@ -4397,7 +4431,7 @@
         <v>5.4</v>
       </c>
       <c r="G74">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="H74">
         <v>5.9</v>
@@ -4409,7 +4443,7 @@
         <v>9</v>
       </c>
       <c r="K74">
-        <v>1.1000000000000001</v>
+        <v>1.1</v>
       </c>
       <c r="L74">
         <v>6.2</v>
@@ -4426,16 +4460,18 @@
       <c r="P74">
         <v>1</v>
       </c>
-      <c r="Q74" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>Jan</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
       <c r="A75">
         <v>6.6</v>
       </c>
       <c r="B75">
-        <v>9.8000000000000007</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C75">
         <v>5.2</v>
@@ -4447,13 +4483,13 @@
         <v>4.8</v>
       </c>
       <c r="F75">
-        <v>5.0999999999999996</v>
+        <v>5.1</v>
       </c>
       <c r="G75">
         <v>5.3</v>
       </c>
       <c r="H75">
-        <v>4.9000000000000004</v>
+        <v>4.9</v>
       </c>
       <c r="I75">
         <v>7.8</v>
@@ -4479,8 +4515,65 @@
       <c r="P75">
         <v>2</v>
       </c>
-      <c r="Q75" t="s">
-        <v>18</v>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>Feb</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76">
+        <v>7.7</v>
+      </c>
+      <c r="B76">
+        <v>9.300000000000001</v>
+      </c>
+      <c r="C76">
+        <v>8.300000000000001</v>
+      </c>
+      <c r="D76">
+        <v>9.4</v>
+      </c>
+      <c r="E76">
+        <v>6.5</v>
+      </c>
+      <c r="F76">
+        <v>5.8</v>
+      </c>
+      <c r="G76">
+        <v>5.7</v>
+      </c>
+      <c r="H76">
+        <v>5.3</v>
+      </c>
+      <c r="I76">
+        <v>1.9</v>
+      </c>
+      <c r="J76">
+        <v>4.4</v>
+      </c>
+      <c r="K76">
+        <v>29.1</v>
+      </c>
+      <c r="L76">
+        <v>7.9</v>
+      </c>
+      <c r="M76">
+        <v>6.3</v>
+      </c>
+      <c r="N76" s="2">
+        <v>44986</v>
+      </c>
+      <c r="O76">
+        <v>2023</v>
+      </c>
+      <c r="P76">
+        <v>3</v>
+      </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>Mar</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>